<commit_message>
08.03.2020 MC SAles Detail
</commit_message>
<xml_diff>
--- a/2020/Others/Target Vs Achivement/DSR wise draft sales target  -Northern-March'2020.xlsx
+++ b/2020/Others/Target Vs Achivement/DSR wise draft sales target  -Northern-March'2020.xlsx
@@ -1715,25 +1715,22 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1746,6 +1743,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2584,7 +2584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2595,10 +2595,10 @@
   <dimension ref="A1:AV29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13002,16 +13002,16 @@
       </c>
     </row>
     <row r="3" spans="1:48" s="23" customFormat="1">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="140" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="140" t="s">
         <v>314</v>
       </c>
       <c r="E3" s="132"/>
@@ -13144,10 +13144,10 @@
       </c>
     </row>
     <row r="4" spans="1:48" s="24" customFormat="1" ht="30">
-      <c r="A4" s="141"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="118" t="s">
         <v>80</v>
       </c>
@@ -13282,7 +13282,7 @@
       </c>
     </row>
     <row r="5" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="141" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -13472,7 +13472,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A6" s="139"/>
+      <c r="A6" s="141"/>
       <c r="B6" s="25" t="s">
         <v>90</v>
       </c>
@@ -13660,7 +13660,7 @@
       </c>
     </row>
     <row r="7" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A7" s="139"/>
+      <c r="A7" s="141"/>
       <c r="B7" s="25" t="s">
         <v>92</v>
       </c>
@@ -13848,7 +13848,7 @@
       </c>
     </row>
     <row r="8" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A8" s="139"/>
+      <c r="A8" s="141"/>
       <c r="B8" s="25" t="s">
         <v>94</v>
       </c>
@@ -14036,7 +14036,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A9" s="139"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="25" t="s">
         <v>96</v>
       </c>
@@ -14224,7 +14224,7 @@
       </c>
     </row>
     <row r="10" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A10" s="139"/>
+      <c r="A10" s="141"/>
       <c r="B10" s="25" t="s">
         <v>98</v>
       </c>
@@ -14412,7 +14412,7 @@
       </c>
     </row>
     <row r="11" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A11" s="139"/>
+      <c r="A11" s="141"/>
       <c r="B11" s="25" t="s">
         <v>100</v>
       </c>
@@ -14600,7 +14600,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A12" s="139"/>
+      <c r="A12" s="141"/>
       <c r="B12" s="25" t="s">
         <v>102</v>
       </c>
@@ -14788,7 +14788,7 @@
       </c>
     </row>
     <row r="13" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A13" s="139" t="s">
+      <c r="A13" s="141" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -14978,7 +14978,7 @@
       </c>
     </row>
     <row r="14" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A14" s="139"/>
+      <c r="A14" s="141"/>
       <c r="B14" s="25" t="s">
         <v>107</v>
       </c>
@@ -15166,7 +15166,7 @@
       </c>
     </row>
     <row r="15" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A15" s="139"/>
+      <c r="A15" s="141"/>
       <c r="B15" s="25" t="s">
         <v>109</v>
       </c>
@@ -15354,7 +15354,7 @@
       </c>
     </row>
     <row r="16" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A16" s="139"/>
+      <c r="A16" s="141"/>
       <c r="B16" s="25" t="s">
         <v>111</v>
       </c>
@@ -18330,7 +18330,7 @@
       <c r="CN28" s="23"/>
     </row>
     <row r="29" spans="1:92" ht="15">
-      <c r="A29" s="138" t="s">
+      <c r="A29" s="139" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="58" t="s">
@@ -18520,7 +18520,7 @@
       </c>
     </row>
     <row r="30" spans="1:92" ht="15">
-      <c r="A30" s="138"/>
+      <c r="A30" s="139"/>
       <c r="B30" s="58" t="s">
         <v>261</v>
       </c>
@@ -18708,7 +18708,7 @@
       </c>
     </row>
     <row r="31" spans="1:92" ht="15">
-      <c r="A31" s="138"/>
+      <c r="A31" s="139"/>
       <c r="B31" s="58" t="s">
         <v>263</v>
       </c>
@@ -18896,7 +18896,7 @@
       </c>
     </row>
     <row r="32" spans="1:92" ht="15">
-      <c r="A32" s="138"/>
+      <c r="A32" s="139"/>
       <c r="B32" s="58" t="s">
         <v>265</v>
       </c>
@@ -19084,7 +19084,7 @@
       </c>
     </row>
     <row r="33" spans="1:48" ht="15">
-      <c r="A33" s="138" t="s">
+      <c r="A33" s="139" t="s">
         <v>267</v>
       </c>
       <c r="B33" s="58" t="s">
@@ -19274,7 +19274,7 @@
       </c>
     </row>
     <row r="34" spans="1:48" ht="15">
-      <c r="A34" s="138"/>
+      <c r="A34" s="139"/>
       <c r="B34" s="58" t="s">
         <v>270</v>
       </c>
@@ -19462,7 +19462,7 @@
       </c>
     </row>
     <row r="35" spans="1:48" ht="15">
-      <c r="A35" s="138"/>
+      <c r="A35" s="139"/>
       <c r="B35" s="58" t="s">
         <v>272</v>
       </c>
@@ -19650,7 +19650,7 @@
       </c>
     </row>
     <row r="36" spans="1:48" ht="15">
-      <c r="A36" s="138" t="s">
+      <c r="A36" s="139" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="67" t="s">
@@ -19840,7 +19840,7 @@
       </c>
     </row>
     <row r="37" spans="1:48" ht="15">
-      <c r="A37" s="138"/>
+      <c r="A37" s="139"/>
       <c r="B37" s="67" t="s">
         <v>234</v>
       </c>
@@ -20028,7 +20028,7 @@
       </c>
     </row>
     <row r="38" spans="1:48" ht="15">
-      <c r="A38" s="138"/>
+      <c r="A38" s="139"/>
       <c r="B38" s="67" t="s">
         <v>236</v>
       </c>
@@ -20216,7 +20216,7 @@
       </c>
     </row>
     <row r="39" spans="1:48" ht="15">
-      <c r="A39" s="138"/>
+      <c r="A39" s="139"/>
       <c r="B39" s="67" t="s">
         <v>238</v>
       </c>
@@ -20404,7 +20404,7 @@
       </c>
     </row>
     <row r="40" spans="1:48" ht="15">
-      <c r="A40" s="138" t="s">
+      <c r="A40" s="139" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="70" t="s">
@@ -20594,7 +20594,7 @@
       </c>
     </row>
     <row r="41" spans="1:48" ht="15">
-      <c r="A41" s="138"/>
+      <c r="A41" s="139"/>
       <c r="B41" s="67" t="s">
         <v>242</v>
       </c>
@@ -20782,7 +20782,7 @@
       </c>
     </row>
     <row r="42" spans="1:48" ht="15">
-      <c r="A42" s="138"/>
+      <c r="A42" s="139"/>
       <c r="B42" s="67" t="s">
         <v>244</v>
       </c>
@@ -20970,7 +20970,7 @@
       </c>
     </row>
     <row r="43" spans="1:48" ht="15">
-      <c r="A43" s="138"/>
+      <c r="A43" s="139"/>
       <c r="B43" s="70" t="s">
         <v>246</v>
       </c>
@@ -21158,7 +21158,7 @@
       </c>
     </row>
     <row r="44" spans="1:48" ht="15">
-      <c r="A44" s="138"/>
+      <c r="A44" s="139"/>
       <c r="B44" s="67" t="s">
         <v>248</v>
       </c>
@@ -21346,7 +21346,7 @@
       </c>
     </row>
     <row r="45" spans="1:48" ht="15">
-      <c r="A45" s="138"/>
+      <c r="A45" s="139"/>
       <c r="B45" s="67" t="s">
         <v>250</v>
       </c>
@@ -21534,7 +21534,7 @@
       </c>
     </row>
     <row r="46" spans="1:48" ht="24.75">
-      <c r="A46" s="138" t="s">
+      <c r="A46" s="139" t="s">
         <v>62</v>
       </c>
       <c r="B46" s="72" t="s">
@@ -21724,7 +21724,7 @@
       </c>
     </row>
     <row r="47" spans="1:48" ht="24.75">
-      <c r="A47" s="138"/>
+      <c r="A47" s="139"/>
       <c r="B47" s="72" t="s">
         <v>280</v>
       </c>
@@ -21912,7 +21912,7 @@
       </c>
     </row>
     <row r="48" spans="1:48" ht="24.75">
-      <c r="A48" s="138"/>
+      <c r="A48" s="139"/>
       <c r="B48" s="72" t="s">
         <v>282</v>
       </c>
@@ -22100,7 +22100,7 @@
       </c>
     </row>
     <row r="49" spans="1:48" ht="24.75">
-      <c r="A49" s="138"/>
+      <c r="A49" s="139"/>
       <c r="B49" s="72" t="s">
         <v>284</v>
       </c>
@@ -22288,7 +22288,7 @@
       </c>
     </row>
     <row r="50" spans="1:48" ht="24.75">
-      <c r="A50" s="138"/>
+      <c r="A50" s="139"/>
       <c r="B50" s="72" t="s">
         <v>286</v>
       </c>
@@ -22476,7 +22476,7 @@
       </c>
     </row>
     <row r="51" spans="1:48" ht="15">
-      <c r="A51" s="138" t="s">
+      <c r="A51" s="139" t="s">
         <v>63</v>
       </c>
       <c r="B51" s="76" t="s">
@@ -22666,7 +22666,7 @@
       </c>
     </row>
     <row r="52" spans="1:48" ht="15">
-      <c r="A52" s="138"/>
+      <c r="A52" s="139"/>
       <c r="B52" s="76" t="s">
         <v>290</v>
       </c>
@@ -22854,7 +22854,7 @@
       </c>
     </row>
     <row r="53" spans="1:48" ht="15">
-      <c r="A53" s="138"/>
+      <c r="A53" s="139"/>
       <c r="B53" s="76" t="s">
         <v>292</v>
       </c>
@@ -23042,7 +23042,7 @@
       </c>
     </row>
     <row r="54" spans="1:48" ht="15">
-      <c r="A54" s="138"/>
+      <c r="A54" s="139"/>
       <c r="B54" s="76" t="s">
         <v>294</v>
       </c>
@@ -23230,7 +23230,7 @@
       </c>
     </row>
     <row r="55" spans="1:48" ht="15">
-      <c r="A55" s="138" t="s">
+      <c r="A55" s="139" t="s">
         <v>64</v>
       </c>
       <c r="B55" s="59" t="s">
@@ -23420,7 +23420,7 @@
       </c>
     </row>
     <row r="56" spans="1:48" ht="15">
-      <c r="A56" s="138"/>
+      <c r="A56" s="139"/>
       <c r="B56" s="59" t="s">
         <v>298</v>
       </c>
@@ -23608,7 +23608,7 @@
       </c>
     </row>
     <row r="57" spans="1:48" ht="15">
-      <c r="A57" s="138"/>
+      <c r="A57" s="139"/>
       <c r="B57" s="59" t="s">
         <v>300</v>
       </c>
@@ -23796,7 +23796,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" ht="15">
-      <c r="A58" s="138"/>
+      <c r="A58" s="139"/>
       <c r="B58" s="59" t="s">
         <v>302</v>
       </c>
@@ -23984,7 +23984,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" ht="15">
-      <c r="A59" s="138"/>
+      <c r="A59" s="139"/>
       <c r="B59" s="59" t="s">
         <v>304</v>
       </c>
@@ -24172,7 +24172,7 @@
       </c>
     </row>
     <row r="60" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A60" s="139" t="s">
+      <c r="A60" s="141" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="25" t="s">
@@ -24362,7 +24362,7 @@
       </c>
     </row>
     <row r="61" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A61" s="139"/>
+      <c r="A61" s="141"/>
       <c r="B61" s="25" t="s">
         <v>175</v>
       </c>
@@ -24550,7 +24550,7 @@
       </c>
     </row>
     <row r="62" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A62" s="139"/>
+      <c r="A62" s="141"/>
       <c r="B62" s="25" t="s">
         <v>177</v>
       </c>
@@ -24738,7 +24738,7 @@
       </c>
     </row>
     <row r="63" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A63" s="139"/>
+      <c r="A63" s="141"/>
       <c r="B63" s="25" t="s">
         <v>179</v>
       </c>
@@ -24926,7 +24926,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A64" s="139" t="s">
+      <c r="A64" s="141" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="25" t="s">
@@ -25116,7 +25116,7 @@
       </c>
     </row>
     <row r="65" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A65" s="139"/>
+      <c r="A65" s="141"/>
       <c r="B65" s="25" t="s">
         <v>183</v>
       </c>
@@ -25304,7 +25304,7 @@
       </c>
     </row>
     <row r="66" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A66" s="139"/>
+      <c r="A66" s="141"/>
       <c r="B66" s="25" t="s">
         <v>185</v>
       </c>
@@ -25492,7 +25492,7 @@
       </c>
     </row>
     <row r="67" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A67" s="139"/>
+      <c r="A67" s="141"/>
       <c r="B67" s="25" t="s">
         <v>187</v>
       </c>
@@ -25680,7 +25680,7 @@
       </c>
     </row>
     <row r="68" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A68" s="139" t="s">
+      <c r="A68" s="141" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="25" t="s">
@@ -25870,7 +25870,7 @@
       </c>
     </row>
     <row r="69" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A69" s="139"/>
+      <c r="A69" s="141"/>
       <c r="B69" s="25" t="s">
         <v>139</v>
       </c>
@@ -26058,7 +26058,7 @@
       </c>
     </row>
     <row r="70" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A70" s="139"/>
+      <c r="A70" s="141"/>
       <c r="B70" s="25" t="s">
         <v>141</v>
       </c>
@@ -26246,7 +26246,7 @@
       </c>
     </row>
     <row r="71" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A71" s="139"/>
+      <c r="A71" s="141"/>
       <c r="B71" s="25" t="s">
         <v>143</v>
       </c>
@@ -26434,7 +26434,7 @@
       </c>
     </row>
     <row r="72" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A72" s="139" t="s">
+      <c r="A72" s="141" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="25" t="s">
@@ -26624,7 +26624,7 @@
       </c>
     </row>
     <row r="73" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A73" s="139"/>
+      <c r="A73" s="141"/>
       <c r="B73" s="25" t="s">
         <v>129</v>
       </c>
@@ -26812,7 +26812,7 @@
       </c>
     </row>
     <row r="74" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A74" s="139"/>
+      <c r="A74" s="141"/>
       <c r="B74" s="25" t="s">
         <v>131</v>
       </c>
@@ -27000,7 +27000,7 @@
       </c>
     </row>
     <row r="75" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A75" s="139"/>
+      <c r="A75" s="141"/>
       <c r="B75" s="25" t="s">
         <v>133</v>
       </c>
@@ -27188,7 +27188,7 @@
       </c>
     </row>
     <row r="76" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A76" s="139"/>
+      <c r="A76" s="141"/>
       <c r="B76" s="25" t="s">
         <v>135</v>
       </c>
@@ -27376,7 +27376,7 @@
       </c>
     </row>
     <row r="77" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A77" s="139" t="s">
+      <c r="A77" s="141" t="s">
         <v>70</v>
       </c>
       <c r="B77" s="25" t="s">
@@ -27566,7 +27566,7 @@
       </c>
     </row>
     <row r="78" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A78" s="139"/>
+      <c r="A78" s="141"/>
       <c r="B78" s="25" t="s">
         <v>123</v>
       </c>
@@ -27754,7 +27754,7 @@
       </c>
     </row>
     <row r="79" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A79" s="139"/>
+      <c r="A79" s="141"/>
       <c r="B79" s="25" t="s">
         <v>125</v>
       </c>
@@ -27942,7 +27942,7 @@
       </c>
     </row>
     <row r="80" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="141" t="s">
         <v>71</v>
       </c>
       <c r="B80" s="25" t="s">
@@ -28132,7 +28132,7 @@
       </c>
     </row>
     <row r="81" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A81" s="139"/>
+      <c r="A81" s="141"/>
       <c r="B81" s="25" t="s">
         <v>147</v>
       </c>
@@ -28320,7 +28320,7 @@
       </c>
     </row>
     <row r="82" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A82" s="139"/>
+      <c r="A82" s="141"/>
       <c r="B82" s="25" t="s">
         <v>149</v>
       </c>
@@ -28508,7 +28508,7 @@
       </c>
     </row>
     <row r="83" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A83" s="139"/>
+      <c r="A83" s="141"/>
       <c r="B83" s="25" t="s">
         <v>151</v>
       </c>
@@ -28696,7 +28696,7 @@
       </c>
     </row>
     <row r="84" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A84" s="139"/>
+      <c r="A84" s="141"/>
       <c r="B84" s="25" t="s">
         <v>153</v>
       </c>
@@ -28884,7 +28884,7 @@
       </c>
     </row>
     <row r="85" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A85" s="139"/>
+      <c r="A85" s="141"/>
       <c r="B85" s="25" t="s">
         <v>155</v>
       </c>
@@ -29072,7 +29072,7 @@
       </c>
     </row>
     <row r="86" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A86" s="139" t="s">
+      <c r="A86" s="141" t="s">
         <v>72</v>
       </c>
       <c r="B86" s="25" t="s">
@@ -29262,7 +29262,7 @@
       </c>
     </row>
     <row r="87" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A87" s="139"/>
+      <c r="A87" s="141"/>
       <c r="B87" s="25" t="s">
         <v>159</v>
       </c>
@@ -29450,7 +29450,7 @@
       </c>
     </row>
     <row r="88" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A88" s="139"/>
+      <c r="A88" s="141"/>
       <c r="B88" s="25" t="s">
         <v>161</v>
       </c>
@@ -29638,7 +29638,7 @@
       </c>
     </row>
     <row r="89" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A89" s="139"/>
+      <c r="A89" s="141"/>
       <c r="B89" s="25" t="s">
         <v>163</v>
       </c>
@@ -29826,7 +29826,7 @@
       </c>
     </row>
     <row r="90" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A90" s="139"/>
+      <c r="A90" s="141"/>
       <c r="B90" s="25" t="s">
         <v>165</v>
       </c>
@@ -30014,7 +30014,7 @@
       </c>
     </row>
     <row r="91" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A91" s="139"/>
+      <c r="A91" s="141"/>
       <c r="B91" s="25" t="s">
         <v>167</v>
       </c>
@@ -30202,7 +30202,7 @@
       </c>
     </row>
     <row r="92" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A92" s="139" t="s">
+      <c r="A92" s="141" t="s">
         <v>73</v>
       </c>
       <c r="B92" s="25" t="s">
@@ -30392,7 +30392,7 @@
       </c>
     </row>
     <row r="93" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A93" s="139"/>
+      <c r="A93" s="141"/>
       <c r="B93" s="25" t="s">
         <v>115</v>
       </c>
@@ -30580,7 +30580,7 @@
       </c>
     </row>
     <row r="94" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A94" s="139"/>
+      <c r="A94" s="141"/>
       <c r="B94" s="25" t="s">
         <v>117</v>
       </c>
@@ -30768,7 +30768,7 @@
       </c>
     </row>
     <row r="95" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A95" s="139"/>
+      <c r="A95" s="141"/>
       <c r="B95" s="25" t="s">
         <v>119</v>
       </c>
@@ -30956,7 +30956,7 @@
       </c>
     </row>
     <row r="96" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A96" s="139" t="s">
+      <c r="A96" s="141" t="s">
         <v>74</v>
       </c>
       <c r="B96" s="25" t="s">
@@ -31146,7 +31146,7 @@
       </c>
     </row>
     <row r="97" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A97" s="139"/>
+      <c r="A97" s="141"/>
       <c r="B97" s="25" t="s">
         <v>169</v>
       </c>
@@ -31334,7 +31334,7 @@
       </c>
     </row>
     <row r="98" spans="1:48" s="23" customFormat="1" ht="15">
-      <c r="A98" s="139"/>
+      <c r="A98" s="141"/>
       <c r="B98" s="25" t="s">
         <v>171</v>
       </c>
@@ -31522,7 +31522,7 @@
       </c>
     </row>
     <row r="99" spans="1:48" ht="15">
-      <c r="A99" s="138" t="s">
+      <c r="A99" s="139" t="s">
         <v>75</v>
       </c>
       <c r="B99" s="58" t="s">
@@ -31712,7 +31712,7 @@
       </c>
     </row>
     <row r="100" spans="1:48" ht="15">
-      <c r="A100" s="138"/>
+      <c r="A100" s="139"/>
       <c r="B100" s="58" t="s">
         <v>216</v>
       </c>
@@ -31900,7 +31900,7 @@
       </c>
     </row>
     <row r="101" spans="1:48" ht="15">
-      <c r="A101" s="138"/>
+      <c r="A101" s="139"/>
       <c r="B101" s="58" t="s">
         <v>218</v>
       </c>
@@ -32088,7 +32088,7 @@
       </c>
     </row>
     <row r="102" spans="1:48" ht="15">
-      <c r="A102" s="138"/>
+      <c r="A102" s="139"/>
       <c r="B102" s="58" t="s">
         <v>220</v>
       </c>
@@ -32276,7 +32276,7 @@
       </c>
     </row>
     <row r="103" spans="1:48" ht="15">
-      <c r="A103" s="138"/>
+      <c r="A103" s="139"/>
       <c r="B103" s="58" t="s">
         <v>222</v>
       </c>
@@ -32464,7 +32464,7 @@
       </c>
     </row>
     <row r="104" spans="1:48" ht="15">
-      <c r="A104" s="138" t="s">
+      <c r="A104" s="139" t="s">
         <v>76</v>
       </c>
       <c r="B104" s="58" t="s">
@@ -32654,7 +32654,7 @@
       </c>
     </row>
     <row r="105" spans="1:48" ht="15">
-      <c r="A105" s="138"/>
+      <c r="A105" s="139"/>
       <c r="B105" s="58" t="s">
         <v>226</v>
       </c>
@@ -32842,7 +32842,7 @@
       </c>
     </row>
     <row r="106" spans="1:48" ht="15">
-      <c r="A106" s="138"/>
+      <c r="A106" s="139"/>
       <c r="B106" s="58" t="s">
         <v>228</v>
       </c>
@@ -33030,7 +33030,7 @@
       </c>
     </row>
     <row r="107" spans="1:48" ht="15">
-      <c r="A107" s="138"/>
+      <c r="A107" s="139"/>
       <c r="B107" s="58" t="s">
         <v>230</v>
       </c>
@@ -33218,7 +33218,7 @@
       </c>
     </row>
     <row r="108" spans="1:48" ht="15">
-      <c r="A108" s="138" t="s">
+      <c r="A108" s="139" t="s">
         <v>252</v>
       </c>
       <c r="B108" s="58" t="s">
@@ -33408,7 +33408,7 @@
       </c>
     </row>
     <row r="109" spans="1:48" ht="15">
-      <c r="A109" s="138"/>
+      <c r="A109" s="139"/>
       <c r="B109" s="58" t="s">
         <v>255</v>
       </c>
@@ -33596,7 +33596,7 @@
       </c>
     </row>
     <row r="110" spans="1:48" ht="15">
-      <c r="A110" s="138"/>
+      <c r="A110" s="139"/>
       <c r="B110" s="58" t="s">
         <v>257</v>
       </c>
@@ -33784,7 +33784,7 @@
       </c>
     </row>
     <row r="111" spans="1:48" ht="15">
-      <c r="A111" s="138" t="s">
+      <c r="A111" s="139" t="s">
         <v>78</v>
       </c>
       <c r="B111" s="58" t="s">
@@ -33974,7 +33974,7 @@
       </c>
     </row>
     <row r="112" spans="1:48" ht="15">
-      <c r="A112" s="138"/>
+      <c r="A112" s="139"/>
       <c r="B112" s="58" t="s">
         <v>276</v>
       </c>
@@ -34162,7 +34162,7 @@
       </c>
     </row>
     <row r="113" spans="1:48" ht="15">
-      <c r="A113" s="138" t="s">
+      <c r="A113" s="139" t="s">
         <v>79</v>
       </c>
       <c r="B113" s="58" t="s">
@@ -34352,7 +34352,7 @@
       </c>
     </row>
     <row r="114" spans="1:48" ht="15">
-      <c r="A114" s="138"/>
+      <c r="A114" s="139"/>
       <c r="B114" s="58" t="s">
         <v>308</v>
       </c>
@@ -34540,7 +34540,7 @@
       </c>
     </row>
     <row r="115" spans="1:48" ht="15">
-      <c r="A115" s="138"/>
+      <c r="A115" s="139"/>
       <c r="B115" s="58" t="s">
         <v>310</v>
       </c>
@@ -34728,7 +34728,7 @@
       </c>
     </row>
     <row r="116" spans="1:48" ht="15">
-      <c r="A116" s="138"/>
+      <c r="A116" s="139"/>
       <c r="B116" s="58" t="s">
         <v>312</v>
       </c>
@@ -34916,12 +34916,12 @@
       </c>
     </row>
     <row r="117" spans="1:48" s="128" customFormat="1">
-      <c r="A117" s="140" t="s">
+      <c r="A117" s="138" t="s">
         <v>315</v>
       </c>
-      <c r="B117" s="140"/>
-      <c r="C117" s="140"/>
-      <c r="D117" s="140"/>
+      <c r="B117" s="138"/>
+      <c r="C117" s="138"/>
+      <c r="D117" s="138"/>
       <c r="E117" s="129">
         <f>SUM(E5:E116)</f>
         <v>209111267.21107674</v>
@@ -35101,6 +35101,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A80:A85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A76"/>
     <mergeCell ref="A117:D117"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A3:A4"/>
@@ -35117,20 +35131,6 @@
     <mergeCell ref="A96:A98"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A80:A85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A99:A103"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:AO3">
     <cfRule type="cellIs" dxfId="55" priority="28" operator="lessThan">
@@ -36882,16 +36882,16 @@
       </c>
     </row>
     <row r="3" spans="1:90" s="23" customFormat="1">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="144" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="145" t="s">
         <v>314</v>
       </c>
       <c r="E3" s="113" t="s">
@@ -37022,10 +37022,10 @@
       </c>
     </row>
     <row r="4" spans="1:90" s="24" customFormat="1" ht="15.75">
-      <c r="A4" s="145"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
+      <c r="A4" s="144"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="112" t="s">
         <v>0</v>
       </c>
@@ -37154,7 +37154,7 @@
       </c>
     </row>
     <row r="5" spans="1:90" s="23" customFormat="1">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="141" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -37294,7 +37294,7 @@
       </c>
     </row>
     <row r="6" spans="1:90" s="23" customFormat="1">
-      <c r="A6" s="139"/>
+      <c r="A6" s="141"/>
       <c r="B6" s="25" t="s">
         <v>90</v>
       </c>
@@ -37432,7 +37432,7 @@
       </c>
     </row>
     <row r="7" spans="1:90" s="23" customFormat="1">
-      <c r="A7" s="139"/>
+      <c r="A7" s="141"/>
       <c r="B7" s="25" t="s">
         <v>92</v>
       </c>
@@ -37570,7 +37570,7 @@
       </c>
     </row>
     <row r="8" spans="1:90" s="23" customFormat="1">
-      <c r="A8" s="139"/>
+      <c r="A8" s="141"/>
       <c r="B8" s="25" t="s">
         <v>94</v>
       </c>
@@ -37708,7 +37708,7 @@
       </c>
     </row>
     <row r="9" spans="1:90" s="23" customFormat="1">
-      <c r="A9" s="139"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="25" t="s">
         <v>96</v>
       </c>
@@ -37846,7 +37846,7 @@
       </c>
     </row>
     <row r="10" spans="1:90" s="23" customFormat="1">
-      <c r="A10" s="139"/>
+      <c r="A10" s="141"/>
       <c r="B10" s="25" t="s">
         <v>98</v>
       </c>
@@ -37984,7 +37984,7 @@
       </c>
     </row>
     <row r="11" spans="1:90" s="23" customFormat="1">
-      <c r="A11" s="139"/>
+      <c r="A11" s="141"/>
       <c r="B11" s="25" t="s">
         <v>100</v>
       </c>
@@ -38122,7 +38122,7 @@
       </c>
     </row>
     <row r="12" spans="1:90" s="23" customFormat="1">
-      <c r="A12" s="139"/>
+      <c r="A12" s="141"/>
       <c r="B12" s="25" t="s">
         <v>102</v>
       </c>
@@ -38436,7 +38436,7 @@
       <c r="CL13" s="23"/>
     </row>
     <row r="14" spans="1:90" s="23" customFormat="1">
-      <c r="A14" s="139" t="s">
+      <c r="A14" s="141" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -38576,7 +38576,7 @@
       </c>
     </row>
     <row r="15" spans="1:90" s="23" customFormat="1">
-      <c r="A15" s="139"/>
+      <c r="A15" s="141"/>
       <c r="B15" s="25" t="s">
         <v>107</v>
       </c>
@@ -38714,7 +38714,7 @@
       </c>
     </row>
     <row r="16" spans="1:90" s="23" customFormat="1">
-      <c r="A16" s="139"/>
+      <c r="A16" s="141"/>
       <c r="B16" s="25" t="s">
         <v>109</v>
       </c>
@@ -38852,7 +38852,7 @@
       </c>
     </row>
     <row r="17" spans="1:90" s="23" customFormat="1">
-      <c r="A17" s="139"/>
+      <c r="A17" s="141"/>
       <c r="B17" s="25" t="s">
         <v>111</v>
       </c>
@@ -41712,7 +41712,7 @@
       <c r="CL32" s="23"/>
     </row>
     <row r="33" spans="1:46">
-      <c r="A33" s="138" t="s">
+      <c r="A33" s="139" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="58" t="s">
@@ -41852,7 +41852,7 @@
       </c>
     </row>
     <row r="34" spans="1:46">
-      <c r="A34" s="138"/>
+      <c r="A34" s="139"/>
       <c r="B34" s="58" t="s">
         <v>261</v>
       </c>
@@ -41990,7 +41990,7 @@
       </c>
     </row>
     <row r="35" spans="1:46">
-      <c r="A35" s="138"/>
+      <c r="A35" s="139"/>
       <c r="B35" s="58" t="s">
         <v>263</v>
       </c>
@@ -42128,7 +42128,7 @@
       </c>
     </row>
     <row r="36" spans="1:46">
-      <c r="A36" s="138"/>
+      <c r="A36" s="139"/>
       <c r="B36" s="58" t="s">
         <v>265</v>
       </c>
@@ -42442,7 +42442,7 @@
       </c>
     </row>
     <row r="38" spans="1:46">
-      <c r="A38" s="138" t="s">
+      <c r="A38" s="139" t="s">
         <v>267</v>
       </c>
       <c r="B38" s="58" t="s">
@@ -42582,7 +42582,7 @@
       </c>
     </row>
     <row r="39" spans="1:46">
-      <c r="A39" s="138"/>
+      <c r="A39" s="139"/>
       <c r="B39" s="58" t="s">
         <v>270</v>
       </c>
@@ -42720,7 +42720,7 @@
       </c>
     </row>
     <row r="40" spans="1:46">
-      <c r="A40" s="138"/>
+      <c r="A40" s="139"/>
       <c r="B40" s="58" t="s">
         <v>272</v>
       </c>
@@ -43034,7 +43034,7 @@
       </c>
     </row>
     <row r="42" spans="1:46">
-      <c r="A42" s="138" t="s">
+      <c r="A42" s="139" t="s">
         <v>59</v>
       </c>
       <c r="B42" s="67" t="s">
@@ -43174,7 +43174,7 @@
       </c>
     </row>
     <row r="43" spans="1:46">
-      <c r="A43" s="138"/>
+      <c r="A43" s="139"/>
       <c r="B43" s="67" t="s">
         <v>234</v>
       </c>
@@ -43312,7 +43312,7 @@
       </c>
     </row>
     <row r="44" spans="1:46">
-      <c r="A44" s="138"/>
+      <c r="A44" s="139"/>
       <c r="B44" s="67" t="s">
         <v>236</v>
       </c>
@@ -43450,7 +43450,7 @@
       </c>
     </row>
     <row r="45" spans="1:46">
-      <c r="A45" s="138"/>
+      <c r="A45" s="139"/>
       <c r="B45" s="67" t="s">
         <v>238</v>
       </c>
@@ -43764,7 +43764,7 @@
       </c>
     </row>
     <row r="47" spans="1:46">
-      <c r="A47" s="144" t="s">
+      <c r="A47" s="148" t="s">
         <v>61</v>
       </c>
       <c r="B47" s="70" t="s">
@@ -43904,7 +43904,7 @@
       </c>
     </row>
     <row r="48" spans="1:46">
-      <c r="A48" s="144"/>
+      <c r="A48" s="148"/>
       <c r="B48" s="67" t="s">
         <v>242</v>
       </c>
@@ -44042,7 +44042,7 @@
       </c>
     </row>
     <row r="49" spans="1:46">
-      <c r="A49" s="144"/>
+      <c r="A49" s="148"/>
       <c r="B49" s="67" t="s">
         <v>244</v>
       </c>
@@ -44180,7 +44180,7 @@
       </c>
     </row>
     <row r="50" spans="1:46">
-      <c r="A50" s="144"/>
+      <c r="A50" s="148"/>
       <c r="B50" s="70" t="s">
         <v>246</v>
       </c>
@@ -44318,7 +44318,7 @@
       </c>
     </row>
     <row r="51" spans="1:46">
-      <c r="A51" s="144"/>
+      <c r="A51" s="148"/>
       <c r="B51" s="67" t="s">
         <v>248</v>
       </c>
@@ -44456,7 +44456,7 @@
       </c>
     </row>
     <row r="52" spans="1:46">
-      <c r="A52" s="144"/>
+      <c r="A52" s="148"/>
       <c r="B52" s="67" t="s">
         <v>250</v>
       </c>
@@ -44770,7 +44770,7 @@
       </c>
     </row>
     <row r="54" spans="1:46" ht="24">
-      <c r="A54" s="138" t="s">
+      <c r="A54" s="139" t="s">
         <v>62</v>
       </c>
       <c r="B54" s="72" t="s">
@@ -44910,7 +44910,7 @@
       </c>
     </row>
     <row r="55" spans="1:46" ht="24">
-      <c r="A55" s="138"/>
+      <c r="A55" s="139"/>
       <c r="B55" s="72" t="s">
         <v>280</v>
       </c>
@@ -45048,7 +45048,7 @@
       </c>
     </row>
     <row r="56" spans="1:46" ht="24">
-      <c r="A56" s="138"/>
+      <c r="A56" s="139"/>
       <c r="B56" s="72" t="s">
         <v>282</v>
       </c>
@@ -45186,7 +45186,7 @@
       </c>
     </row>
     <row r="57" spans="1:46" ht="24">
-      <c r="A57" s="138"/>
+      <c r="A57" s="139"/>
       <c r="B57" s="72" t="s">
         <v>284</v>
       </c>
@@ -45324,7 +45324,7 @@
       </c>
     </row>
     <row r="58" spans="1:46" ht="24">
-      <c r="A58" s="138"/>
+      <c r="A58" s="139"/>
       <c r="B58" s="72" t="s">
         <v>286</v>
       </c>
@@ -45638,7 +45638,7 @@
       </c>
     </row>
     <row r="60" spans="1:46">
-      <c r="A60" s="138" t="s">
+      <c r="A60" s="139" t="s">
         <v>63</v>
       </c>
       <c r="B60" s="76" t="s">
@@ -45778,7 +45778,7 @@
       </c>
     </row>
     <row r="61" spans="1:46">
-      <c r="A61" s="138"/>
+      <c r="A61" s="139"/>
       <c r="B61" s="76" t="s">
         <v>290</v>
       </c>
@@ -45916,7 +45916,7 @@
       </c>
     </row>
     <row r="62" spans="1:46">
-      <c r="A62" s="138"/>
+      <c r="A62" s="139"/>
       <c r="B62" s="76" t="s">
         <v>292</v>
       </c>
@@ -46054,7 +46054,7 @@
       </c>
     </row>
     <row r="63" spans="1:46">
-      <c r="A63" s="138"/>
+      <c r="A63" s="139"/>
       <c r="B63" s="76" t="s">
         <v>294</v>
       </c>
@@ -46368,7 +46368,7 @@
       </c>
     </row>
     <row r="65" spans="1:90">
-      <c r="A65" s="138" t="s">
+      <c r="A65" s="139" t="s">
         <v>64</v>
       </c>
       <c r="B65" s="59" t="s">
@@ -46508,7 +46508,7 @@
       </c>
     </row>
     <row r="66" spans="1:90">
-      <c r="A66" s="138"/>
+      <c r="A66" s="139"/>
       <c r="B66" s="59" t="s">
         <v>298</v>
       </c>
@@ -46646,7 +46646,7 @@
       </c>
     </row>
     <row r="67" spans="1:90">
-      <c r="A67" s="138"/>
+      <c r="A67" s="139"/>
       <c r="B67" s="59" t="s">
         <v>300</v>
       </c>
@@ -46784,7 +46784,7 @@
       </c>
     </row>
     <row r="68" spans="1:90">
-      <c r="A68" s="138"/>
+      <c r="A68" s="139"/>
       <c r="B68" s="59" t="s">
         <v>302</v>
       </c>
@@ -46922,7 +46922,7 @@
       </c>
     </row>
     <row r="69" spans="1:90">
-      <c r="A69" s="138"/>
+      <c r="A69" s="139"/>
       <c r="B69" s="59" t="s">
         <v>304</v>
       </c>
@@ -47236,7 +47236,7 @@
       </c>
     </row>
     <row r="71" spans="1:90" s="23" customFormat="1">
-      <c r="A71" s="139" t="s">
+      <c r="A71" s="141" t="s">
         <v>65</v>
       </c>
       <c r="B71" s="25" t="s">
@@ -47376,7 +47376,7 @@
       </c>
     </row>
     <row r="72" spans="1:90" s="23" customFormat="1">
-      <c r="A72" s="139"/>
+      <c r="A72" s="141"/>
       <c r="B72" s="25" t="s">
         <v>175</v>
       </c>
@@ -47514,7 +47514,7 @@
       </c>
     </row>
     <row r="73" spans="1:90" s="23" customFormat="1">
-      <c r="A73" s="139"/>
+      <c r="A73" s="141"/>
       <c r="B73" s="25" t="s">
         <v>177</v>
       </c>
@@ -47652,7 +47652,7 @@
       </c>
     </row>
     <row r="74" spans="1:90" s="23" customFormat="1">
-      <c r="A74" s="139"/>
+      <c r="A74" s="141"/>
       <c r="B74" s="25" t="s">
         <v>179</v>
       </c>
@@ -47968,7 +47968,7 @@
       <c r="CL75" s="23"/>
     </row>
     <row r="76" spans="1:90" s="23" customFormat="1">
-      <c r="A76" s="139" t="s">
+      <c r="A76" s="141" t="s">
         <v>67</v>
       </c>
       <c r="B76" s="25" t="s">
@@ -48108,7 +48108,7 @@
       </c>
     </row>
     <row r="77" spans="1:90" s="23" customFormat="1">
-      <c r="A77" s="139"/>
+      <c r="A77" s="141"/>
       <c r="B77" s="25" t="s">
         <v>183</v>
       </c>
@@ -48246,7 +48246,7 @@
       </c>
     </row>
     <row r="78" spans="1:90" s="23" customFormat="1">
-      <c r="A78" s="139"/>
+      <c r="A78" s="141"/>
       <c r="B78" s="25" t="s">
         <v>185</v>
       </c>
@@ -48384,7 +48384,7 @@
       </c>
     </row>
     <row r="79" spans="1:90" s="23" customFormat="1">
-      <c r="A79" s="139"/>
+      <c r="A79" s="141"/>
       <c r="B79" s="25" t="s">
         <v>187</v>
       </c>
@@ -48700,7 +48700,7 @@
       <c r="CL80" s="23"/>
     </row>
     <row r="81" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A81" s="139" t="s">
+      <c r="A81" s="141" t="s">
         <v>68</v>
       </c>
       <c r="B81" s="25" t="s">
@@ -48840,7 +48840,7 @@
       </c>
     </row>
     <row r="82" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A82" s="139"/>
+      <c r="A82" s="141"/>
       <c r="B82" s="25" t="s">
         <v>139</v>
       </c>
@@ -48978,7 +48978,7 @@
       </c>
     </row>
     <row r="83" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="139"/>
+      <c r="A83" s="141"/>
       <c r="B83" s="25" t="s">
         <v>141</v>
       </c>
@@ -49116,7 +49116,7 @@
       </c>
     </row>
     <row r="84" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="139"/>
+      <c r="A84" s="141"/>
       <c r="B84" s="25" t="s">
         <v>143</v>
       </c>
@@ -49432,7 +49432,7 @@
       <c r="CL85" s="23"/>
     </row>
     <row r="86" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A86" s="139" t="s">
+      <c r="A86" s="141" t="s">
         <v>69</v>
       </c>
       <c r="B86" s="25" t="s">
@@ -49572,7 +49572,7 @@
       </c>
     </row>
     <row r="87" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A87" s="139"/>
+      <c r="A87" s="141"/>
       <c r="B87" s="25" t="s">
         <v>129</v>
       </c>
@@ -49710,7 +49710,7 @@
       </c>
     </row>
     <row r="88" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="139"/>
+      <c r="A88" s="141"/>
       <c r="B88" s="25" t="s">
         <v>131</v>
       </c>
@@ -49848,7 +49848,7 @@
       </c>
     </row>
     <row r="89" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A89" s="139"/>
+      <c r="A89" s="141"/>
       <c r="B89" s="25" t="s">
         <v>133</v>
       </c>
@@ -49986,7 +49986,7 @@
       </c>
     </row>
     <row r="90" spans="1:90" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A90" s="139"/>
+      <c r="A90" s="141"/>
       <c r="B90" s="25" t="s">
         <v>135</v>
       </c>
@@ -50258,7 +50258,7 @@
       </c>
     </row>
     <row r="92" spans="1:90" s="23" customFormat="1">
-      <c r="A92" s="139" t="s">
+      <c r="A92" s="141" t="s">
         <v>70</v>
       </c>
       <c r="B92" s="25" t="s">
@@ -50398,7 +50398,7 @@
       </c>
     </row>
     <row r="93" spans="1:90" s="23" customFormat="1">
-      <c r="A93" s="139"/>
+      <c r="A93" s="141"/>
       <c r="B93" s="25" t="s">
         <v>123</v>
       </c>
@@ -50536,7 +50536,7 @@
       </c>
     </row>
     <row r="94" spans="1:90" s="23" customFormat="1">
-      <c r="A94" s="139"/>
+      <c r="A94" s="141"/>
       <c r="B94" s="25" t="s">
         <v>125</v>
       </c>
@@ -50852,7 +50852,7 @@
       <c r="CL95" s="23"/>
     </row>
     <row r="96" spans="1:90" s="23" customFormat="1">
-      <c r="A96" s="139" t="s">
+      <c r="A96" s="141" t="s">
         <v>71</v>
       </c>
       <c r="B96" s="25" t="s">
@@ -50992,7 +50992,7 @@
       </c>
     </row>
     <row r="97" spans="1:90" s="23" customFormat="1">
-      <c r="A97" s="139"/>
+      <c r="A97" s="141"/>
       <c r="B97" s="25" t="s">
         <v>147</v>
       </c>
@@ -51130,7 +51130,7 @@
       </c>
     </row>
     <row r="98" spans="1:90" s="23" customFormat="1">
-      <c r="A98" s="139"/>
+      <c r="A98" s="141"/>
       <c r="B98" s="25" t="s">
         <v>149</v>
       </c>
@@ -51268,7 +51268,7 @@
       </c>
     </row>
     <row r="99" spans="1:90" s="23" customFormat="1">
-      <c r="A99" s="139"/>
+      <c r="A99" s="141"/>
       <c r="B99" s="25" t="s">
         <v>151</v>
       </c>
@@ -51406,7 +51406,7 @@
       </c>
     </row>
     <row r="100" spans="1:90" s="23" customFormat="1">
-      <c r="A100" s="139"/>
+      <c r="A100" s="141"/>
       <c r="B100" s="25" t="s">
         <v>153</v>
       </c>
@@ -51544,7 +51544,7 @@
       </c>
     </row>
     <row r="101" spans="1:90" s="23" customFormat="1">
-      <c r="A101" s="139"/>
+      <c r="A101" s="141"/>
       <c r="B101" s="25" t="s">
         <v>155</v>
       </c>
@@ -51860,7 +51860,7 @@
       <c r="CL102" s="23"/>
     </row>
     <row r="103" spans="1:90" s="23" customFormat="1">
-      <c r="A103" s="139" t="s">
+      <c r="A103" s="141" t="s">
         <v>72</v>
       </c>
       <c r="B103" s="25" t="s">
@@ -52000,7 +52000,7 @@
       </c>
     </row>
     <row r="104" spans="1:90" s="23" customFormat="1">
-      <c r="A104" s="139"/>
+      <c r="A104" s="141"/>
       <c r="B104" s="25" t="s">
         <v>159</v>
       </c>
@@ -52138,7 +52138,7 @@
       </c>
     </row>
     <row r="105" spans="1:90" s="23" customFormat="1">
-      <c r="A105" s="139"/>
+      <c r="A105" s="141"/>
       <c r="B105" s="25" t="s">
         <v>161</v>
       </c>
@@ -52276,7 +52276,7 @@
       </c>
     </row>
     <row r="106" spans="1:90" s="23" customFormat="1">
-      <c r="A106" s="139"/>
+      <c r="A106" s="141"/>
       <c r="B106" s="25" t="s">
         <v>163</v>
       </c>
@@ -52414,7 +52414,7 @@
       </c>
     </row>
     <row r="107" spans="1:90" s="23" customFormat="1">
-      <c r="A107" s="139"/>
+      <c r="A107" s="141"/>
       <c r="B107" s="25" t="s">
         <v>165</v>
       </c>
@@ -52552,7 +52552,7 @@
       </c>
     </row>
     <row r="108" spans="1:90" s="23" customFormat="1">
-      <c r="A108" s="139"/>
+      <c r="A108" s="141"/>
       <c r="B108" s="25" t="s">
         <v>167</v>
       </c>
@@ -52868,7 +52868,7 @@
       <c r="CL109" s="23"/>
     </row>
     <row r="110" spans="1:90" s="23" customFormat="1">
-      <c r="A110" s="139" t="s">
+      <c r="A110" s="141" t="s">
         <v>73</v>
       </c>
       <c r="B110" s="25" t="s">
@@ -53008,7 +53008,7 @@
       </c>
     </row>
     <row r="111" spans="1:90" s="23" customFormat="1">
-      <c r="A111" s="139"/>
+      <c r="A111" s="141"/>
       <c r="B111" s="25" t="s">
         <v>115</v>
       </c>
@@ -53146,7 +53146,7 @@
       </c>
     </row>
     <row r="112" spans="1:90" s="23" customFormat="1">
-      <c r="A112" s="139"/>
+      <c r="A112" s="141"/>
       <c r="B112" s="25" t="s">
         <v>117</v>
       </c>
@@ -53284,7 +53284,7 @@
       </c>
     </row>
     <row r="113" spans="1:90" s="23" customFormat="1">
-      <c r="A113" s="139"/>
+      <c r="A113" s="141"/>
       <c r="B113" s="25" t="s">
         <v>119</v>
       </c>
@@ -53600,7 +53600,7 @@
       <c r="CL114" s="23"/>
     </row>
     <row r="115" spans="1:90" s="23" customFormat="1">
-      <c r="A115" s="139" t="s">
+      <c r="A115" s="141" t="s">
         <v>74</v>
       </c>
       <c r="B115" s="25" t="s">
@@ -53740,7 +53740,7 @@
       </c>
     </row>
     <row r="116" spans="1:90" s="23" customFormat="1">
-      <c r="A116" s="139"/>
+      <c r="A116" s="141"/>
       <c r="B116" s="25" t="s">
         <v>169</v>
       </c>
@@ -53878,7 +53878,7 @@
       </c>
     </row>
     <row r="117" spans="1:90" s="23" customFormat="1">
-      <c r="A117" s="139"/>
+      <c r="A117" s="141"/>
       <c r="B117" s="25" t="s">
         <v>171</v>
       </c>
@@ -54194,7 +54194,7 @@
       <c r="CL118" s="23"/>
     </row>
     <row r="119" spans="1:90">
-      <c r="A119" s="138" t="s">
+      <c r="A119" s="139" t="s">
         <v>75</v>
       </c>
       <c r="B119" s="58" t="s">
@@ -54334,7 +54334,7 @@
       </c>
     </row>
     <row r="120" spans="1:90">
-      <c r="A120" s="138"/>
+      <c r="A120" s="139"/>
       <c r="B120" s="58" t="s">
         <v>216</v>
       </c>
@@ -54472,7 +54472,7 @@
       </c>
     </row>
     <row r="121" spans="1:90">
-      <c r="A121" s="138"/>
+      <c r="A121" s="139"/>
       <c r="B121" s="58" t="s">
         <v>218</v>
       </c>
@@ -54610,7 +54610,7 @@
       </c>
     </row>
     <row r="122" spans="1:90">
-      <c r="A122" s="138"/>
+      <c r="A122" s="139"/>
       <c r="B122" s="58" t="s">
         <v>220</v>
       </c>
@@ -54748,7 +54748,7 @@
       </c>
     </row>
     <row r="123" spans="1:90">
-      <c r="A123" s="138"/>
+      <c r="A123" s="139"/>
       <c r="B123" s="58" t="s">
         <v>222</v>
       </c>
@@ -55062,7 +55062,7 @@
       </c>
     </row>
     <row r="125" spans="1:90">
-      <c r="A125" s="138" t="s">
+      <c r="A125" s="139" t="s">
         <v>76</v>
       </c>
       <c r="B125" s="58" t="s">
@@ -55202,7 +55202,7 @@
       </c>
     </row>
     <row r="126" spans="1:90">
-      <c r="A126" s="138"/>
+      <c r="A126" s="139"/>
       <c r="B126" s="58" t="s">
         <v>226</v>
       </c>
@@ -55340,7 +55340,7 @@
       </c>
     </row>
     <row r="127" spans="1:90">
-      <c r="A127" s="138"/>
+      <c r="A127" s="139"/>
       <c r="B127" s="58" t="s">
         <v>228</v>
       </c>
@@ -55478,7 +55478,7 @@
       </c>
     </row>
     <row r="128" spans="1:90">
-      <c r="A128" s="138"/>
+      <c r="A128" s="139"/>
       <c r="B128" s="58" t="s">
         <v>230</v>
       </c>
@@ -55792,7 +55792,7 @@
       </c>
     </row>
     <row r="130" spans="1:46">
-      <c r="A130" s="138" t="s">
+      <c r="A130" s="139" t="s">
         <v>252</v>
       </c>
       <c r="B130" s="58" t="s">
@@ -55932,7 +55932,7 @@
       </c>
     </row>
     <row r="131" spans="1:46">
-      <c r="A131" s="138"/>
+      <c r="A131" s="139"/>
       <c r="B131" s="58" t="s">
         <v>255</v>
       </c>
@@ -56070,7 +56070,7 @@
       </c>
     </row>
     <row r="132" spans="1:46">
-      <c r="A132" s="138"/>
+      <c r="A132" s="139"/>
       <c r="B132" s="58" t="s">
         <v>257</v>
       </c>
@@ -56384,7 +56384,7 @@
       </c>
     </row>
     <row r="134" spans="1:46">
-      <c r="A134" s="138" t="s">
+      <c r="A134" s="139" t="s">
         <v>78</v>
       </c>
       <c r="B134" s="58" t="s">
@@ -56524,7 +56524,7 @@
       </c>
     </row>
     <row r="135" spans="1:46">
-      <c r="A135" s="138"/>
+      <c r="A135" s="139"/>
       <c r="B135" s="58" t="s">
         <v>276</v>
       </c>
@@ -56838,7 +56838,7 @@
       </c>
     </row>
     <row r="137" spans="1:46">
-      <c r="A137" s="138" t="s">
+      <c r="A137" s="139" t="s">
         <v>79</v>
       </c>
       <c r="B137" s="58" t="s">
@@ -56978,7 +56978,7 @@
       </c>
     </row>
     <row r="138" spans="1:46">
-      <c r="A138" s="138"/>
+      <c r="A138" s="139"/>
       <c r="B138" s="58" t="s">
         <v>308</v>
       </c>
@@ -57116,7 +57116,7 @@
       </c>
     </row>
     <row r="139" spans="1:46">
-      <c r="A139" s="138"/>
+      <c r="A139" s="139"/>
       <c r="B139" s="58" t="s">
         <v>310</v>
       </c>
@@ -57254,7 +57254,7 @@
       </c>
     </row>
     <row r="140" spans="1:46">
-      <c r="A140" s="138"/>
+      <c r="A140" s="139"/>
       <c r="B140" s="58" t="s">
         <v>312</v>
       </c>
@@ -57569,6 +57569,21 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A137:A140"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:A12"/>
     <mergeCell ref="A115:A117"/>
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A76:A79"/>
@@ -57583,21 +57598,6 @@
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A137:A140"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AM3">
     <cfRule type="cellIs" dxfId="51" priority="52" operator="lessThan">

</xml_diff>